<commit_message>
feat: se crea circuito para valor 9 desde chatgpt en word
</commit_message>
<xml_diff>
--- a/Yupana5-sumador-base-10.xlsx
+++ b/Yupana5-sumador-base-10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a5cacf8b017db50b/Documentos/Investigacion/Yupanas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1016" documentId="8_{B9B11355-E9F0-4463-8955-61DA98F53D81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{47CE7CB4-CDDD-446A-86FD-936F51E791AD}"/>
+  <xr:revisionPtr revIDLastSave="1021" documentId="8_{B9B11355-E9F0-4463-8955-61DA98F53D81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{A74B5BC5-0B76-4A05-ABFE-99018F0F6E80}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="740" firstSheet="6" activeTab="22" xr2:uid="{D1CB58D7-3A52-4FB2-84EC-43028C6ACB24}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="740" firstSheet="10" activeTab="22" xr2:uid="{D1CB58D7-3A52-4FB2-84EC-43028C6ACB24}"/>
   </bookViews>
   <sheets>
     <sheet name="Representación" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,8 @@
     <sheet name="#4-&gt; 6" sheetId="21" r:id="rId20"/>
     <sheet name="#3-&gt; 7" sheetId="22" r:id="rId21"/>
     <sheet name="#2-&gt; 8" sheetId="23" r:id="rId22"/>
-    <sheet name="#2-&gt; 9" sheetId="24" r:id="rId23"/>
+    <sheet name="#1-&gt; 9" sheetId="24" r:id="rId23"/>
+    <sheet name="Hoja1" sheetId="25" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="60">
   <si>
     <t>respuesta</t>
   </si>
@@ -32147,7 +32148,7 @@
   <dimension ref="A1:AO25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="AN4" sqref="AN4:AN24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33588,6 +33589,441 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07079819-4B40-4307-B60F-B07CA5E520BA}">
+  <dimension ref="B5:G25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="5">
+        <v>0</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="5">
+        <v>0</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="5">
+        <v>0</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1</v>
+      </c>
+      <c r="E22" s="5">
+        <v>1</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0</v>
+      </c>
+      <c r="G22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="5">
+        <v>0</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1</v>
+      </c>
+      <c r="E23" s="5">
+        <v>1</v>
+      </c>
+      <c r="F23" s="5">
+        <v>1</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="5">
+        <v>0</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="5">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <v>1</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>